<commit_message>
dhan bahadur complete and bibha mijar complete and before going to hospital at gangalaal
</commit_message>
<xml_diff>
--- a/ofc/estimates/सेतिदेवी मन्दिर संरक्षण/सेतिदेवी मन्दिर संरक्षण.xlsx
+++ b/ofc/estimates/सेतिदेवी मन्दिर संरक्षण/सेतिदेवी मन्दिर संरक्षण.xlsx
@@ -9,23 +9,25 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="WCR" sheetId="6" r:id="rId1"/>
     <sheet name="Estimate (3)" sheetId="19" r:id="rId2"/>
     <sheet name="plum" sheetId="20" r:id="rId3"/>
+    <sheet name="manual excavation" sheetId="21" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
     <externalReference r:id="rId7"/>
     <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
   </externalReferences>
   <definedNames>
     <definedName name="description_103">[1]Abstract!$B$16</definedName>
     <definedName name="description_124" localSheetId="1">#REF!</definedName>
+    <definedName name="description_124" localSheetId="3">#REF!</definedName>
     <definedName name="description_124" localSheetId="2">#REF!</definedName>
     <definedName name="description_124">#REF!</definedName>
     <definedName name="description_247">[1]Abstract!$B$22</definedName>
@@ -41,8 +43,10 @@
     <definedName name="description_781">[5]Abstract!$B$299</definedName>
     <definedName name="description_783">[1]Abstract!$B$301</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Estimate (3)'!$A$1:$K$43</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'manual excavation'!$A$1:$K$42</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">plum!$A$1:$K$43</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Estimate (3)'!$1:$8</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="3">'manual excavation'!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">plum!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">WCR!$1:$12</definedName>
   </definedNames>
@@ -64,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="60">
   <si>
     <t>Government of Nepal</t>
   </si>
@@ -241,6 +245,9 @@
   </si>
   <si>
     <t>Date:2081/09/29</t>
+  </si>
+  <si>
+    <t>Earthwork Excavation in Cutting., Roadway Excavation in all types of Soil by Manual Means ., Roadway Excavation in all types of soil as per drawing and technical specification, including removal of stumps and other deleterious matter, with all lifts and lead as per Drawing and instruction of the Engineer.</t>
   </si>
 </sst>
 </file>
@@ -559,6 +566,24 @@
     <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -583,22 +608,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -610,18 +629,6 @@
     </xf>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1261,90 +1268,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
     </row>
     <row r="2" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="78"/>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="70"/>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="78"/>
-      <c r="K4" s="78"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="70"/>
     </row>
     <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="79" t="s">
+      <c r="A5" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="79"/>
-      <c r="C5" s="79"/>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
-      <c r="G5" s="79"/>
-      <c r="H5" s="79"/>
-      <c r="I5" s="79"/>
-      <c r="J5" s="79"/>
-      <c r="K5" s="79"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="71"/>
+      <c r="K5" s="71"/>
     </row>
     <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="74" t="e">
+      <c r="C6" s="66" t="e">
         <f>F18</f>
         <v>#REF!</v>
       </c>
-      <c r="D6" s="75"/>
+      <c r="D6" s="67"/>
       <c r="E6" s="9"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -1352,11 +1359,11 @@
         <v>20</v>
       </c>
       <c r="I6" s="8"/>
-      <c r="J6" s="74" t="e">
+      <c r="J6" s="66" t="e">
         <f>I18</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="75"/>
+      <c r="K6" s="67"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
@@ -1365,77 +1372,77 @@
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
-      <c r="I7" s="70" t="s">
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
+      <c r="I7" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="70"/>
-      <c r="K7" s="70"/>
+      <c r="J7" s="76"/>
+      <c r="K7" s="76"/>
     </row>
     <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="68" t="e">
+      <c r="A8" s="74" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="68"/>
-      <c r="I8" s="71" t="s">
+      <c r="B8" s="74"/>
+      <c r="C8" s="74"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="74"/>
+      <c r="I8" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="71"/>
-      <c r="K8" s="71"/>
+      <c r="J8" s="77"/>
+      <c r="K8" s="77"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="72" t="e">
+      <c r="A9" s="78" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B9" s="72"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="I9" s="71" t="s">
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="78"/>
+      <c r="I9" s="77" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="71"/>
-      <c r="K9" s="71"/>
+      <c r="J9" s="77"/>
+      <c r="K9" s="77"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="66" t="s">
+      <c r="A11" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="66" t="s">
+      <c r="B11" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="66" t="s">
+      <c r="C11" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="73" t="s">
+      <c r="D11" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73"/>
-      <c r="G11" s="73" t="s">
+      <c r="E11" s="79"/>
+      <c r="F11" s="79"/>
+      <c r="G11" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="73"/>
-      <c r="I11" s="73"/>
-      <c r="J11" s="66" t="s">
+      <c r="H11" s="79"/>
+      <c r="I11" s="79"/>
+      <c r="J11" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="67" t="s">
+      <c r="K11" s="73" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="66"/>
-      <c r="B12" s="66"/>
-      <c r="C12" s="66"/>
+      <c r="A12" s="72"/>
+      <c r="B12" s="72"/>
+      <c r="C12" s="72"/>
       <c r="D12" s="11" t="s">
         <v>26</v>
       </c>
@@ -1454,8 +1461,8 @@
       <c r="I12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="66"/>
-      <c r="K12" s="67"/>
+      <c r="J12" s="72"/>
+      <c r="K12" s="73"/>
     </row>
     <row r="13" spans="1:11" s="1" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A13" s="27" t="e">
@@ -1617,13 +1624,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -1637,6 +1637,13 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1654,7 +1661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S100"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -1673,116 +1680,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="85"/>
-      <c r="J1" s="85"/>
-      <c r="K1" s="85"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="82"/>
     </row>
     <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="78"/>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="70"/>
     </row>
     <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="78"/>
-      <c r="K4" s="78"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="70"/>
     </row>
     <row r="5" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="87" t="s">
+      <c r="A5" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="87"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="87"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="87"/>
-      <c r="H5" s="87"/>
-      <c r="I5" s="87"/>
-      <c r="J5" s="87"/>
-      <c r="K5" s="87"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="83"/>
     </row>
     <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="68" t="s">
+      <c r="A6" s="74" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="68"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
+      <c r="B6" s="74"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="74"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="74"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="84" t="s">
+      <c r="H6" s="80" t="s">
         <v>46</v>
       </c>
-      <c r="I6" s="84"/>
-      <c r="J6" s="84"/>
-      <c r="K6" s="84"/>
+      <c r="I6" s="80"/>
+      <c r="J6" s="80"/>
+      <c r="K6" s="80"/>
       <c r="O6" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="81" t="s">
+      <c r="A7" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="81"/>
-      <c r="C7" s="81"/>
-      <c r="D7" s="81"/>
-      <c r="E7" s="81"/>
-      <c r="F7" s="81"/>
+      <c r="B7" s="85"/>
+      <c r="C7" s="85"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="85"/>
+      <c r="F7" s="85"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="82" t="s">
+      <c r="H7" s="86" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="82"/>
-      <c r="J7" s="82"/>
-      <c r="K7" s="82"/>
+      <c r="I7" s="86"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="86"/>
     </row>
     <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -2531,11 +2538,11 @@
       <c r="B38" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="80">
+      <c r="C38" s="84">
         <f>J36</f>
         <v>561973.027367</v>
       </c>
-      <c r="D38" s="80"/>
+      <c r="D38" s="84"/>
       <c r="E38" s="40">
         <v>100</v>
       </c>
@@ -2551,10 +2558,10 @@
       <c r="B39" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C39" s="83">
+      <c r="C39" s="87">
         <v>500000</v>
       </c>
-      <c r="D39" s="83"/>
+      <c r="D39" s="87"/>
       <c r="E39" s="40"/>
       <c r="F39" s="50"/>
       <c r="G39" s="49"/>
@@ -2568,11 +2575,11 @@
       <c r="B40" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C40" s="83">
+      <c r="C40" s="87">
         <f>C39-C42-C43</f>
         <v>475000</v>
       </c>
-      <c r="D40" s="83"/>
+      <c r="D40" s="87"/>
       <c r="E40" s="40">
         <f>C40/C38*100</f>
         <v>84.52362958156678</v>
@@ -2589,11 +2596,11 @@
       <c r="B41" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C41" s="80">
+      <c r="C41" s="84">
         <f>C38-C40</f>
         <v>86973.027367000002</v>
       </c>
-      <c r="D41" s="80"/>
+      <c r="D41" s="84"/>
       <c r="E41" s="40">
         <f>100-E40</f>
         <v>15.47637041843322</v>
@@ -2610,11 +2617,11 @@
       <c r="B42" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C42" s="80">
+      <c r="C42" s="84">
         <f>C39*0.03</f>
         <v>15000</v>
       </c>
-      <c r="D42" s="80"/>
+      <c r="D42" s="84"/>
       <c r="E42" s="40">
         <v>3</v>
       </c>
@@ -2630,11 +2637,11 @@
       <c r="B43" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C43" s="80">
+      <c r="C43" s="84">
         <f>C39*0.02</f>
         <v>10000</v>
       </c>
-      <c r="D43" s="80"/>
+      <c r="D43" s="84"/>
       <c r="E43" s="40">
         <v>2</v>
       </c>
@@ -2716,13 +2723,6 @@
     <row r="100" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C42:D42"/>
     <mergeCell ref="C43:D43"/>
     <mergeCell ref="A7:F7"/>
@@ -2731,6 +2731,13 @@
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="C41:D41"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
@@ -2744,8 +2751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S100"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A20" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2763,116 +2770,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="85"/>
-      <c r="J1" s="85"/>
-      <c r="K1" s="85"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="82"/>
     </row>
     <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="78"/>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="70"/>
     </row>
     <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="78"/>
-      <c r="K4" s="78"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="70"/>
     </row>
     <row r="5" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="87" t="s">
+      <c r="A5" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="87"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="87"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="87"/>
-      <c r="H5" s="87"/>
-      <c r="I5" s="87"/>
-      <c r="J5" s="87"/>
-      <c r="K5" s="87"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="83"/>
     </row>
     <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="68" t="s">
+      <c r="A6" s="74" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="68"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
+      <c r="B6" s="74"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="74"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="74"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="84" t="s">
+      <c r="H6" s="80" t="s">
         <v>46</v>
       </c>
-      <c r="I6" s="84"/>
-      <c r="J6" s="84"/>
-      <c r="K6" s="84"/>
+      <c r="I6" s="80"/>
+      <c r="J6" s="80"/>
+      <c r="K6" s="80"/>
       <c r="O6" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="81" t="s">
+      <c r="A7" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="81"/>
-      <c r="C7" s="81"/>
-      <c r="D7" s="81"/>
-      <c r="E7" s="81"/>
-      <c r="F7" s="81"/>
+      <c r="B7" s="85"/>
+      <c r="C7" s="85"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="85"/>
+      <c r="F7" s="85"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="82" t="s">
+      <c r="H7" s="86" t="s">
         <v>58</v>
       </c>
-      <c r="I7" s="82"/>
-      <c r="J7" s="82"/>
-      <c r="K7" s="82"/>
+      <c r="I7" s="86"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="86"/>
     </row>
     <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -3621,11 +3628,11 @@
       <c r="B38" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="80">
+      <c r="C38" s="84">
         <f>J36</f>
         <v>563450.73468724987</v>
       </c>
-      <c r="D38" s="80"/>
+      <c r="D38" s="84"/>
       <c r="E38" s="40">
         <v>100</v>
       </c>
@@ -3641,10 +3648,10 @@
       <c r="B39" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C39" s="83">
+      <c r="C39" s="87">
         <v>500000</v>
       </c>
-      <c r="D39" s="83"/>
+      <c r="D39" s="87"/>
       <c r="E39" s="40"/>
       <c r="F39" s="50"/>
       <c r="G39" s="49"/>
@@ -3658,11 +3665,11 @@
       <c r="B40" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C40" s="83">
+      <c r="C40" s="87">
         <f>C39-C42-C43</f>
         <v>475000</v>
       </c>
-      <c r="D40" s="83"/>
+      <c r="D40" s="87"/>
       <c r="E40" s="40">
         <f>C40/C38*100</f>
         <v>84.301957697092092</v>
@@ -3679,11 +3686,11 @@
       <c r="B41" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C41" s="80">
+      <c r="C41" s="84">
         <f>C38-C40</f>
         <v>88450.734687249875</v>
       </c>
-      <c r="D41" s="80"/>
+      <c r="D41" s="84"/>
       <c r="E41" s="40">
         <f>100-E40</f>
         <v>15.698042302907908</v>
@@ -3700,11 +3707,11 @@
       <c r="B42" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C42" s="80">
+      <c r="C42" s="84">
         <f>C39*0.03</f>
         <v>15000</v>
       </c>
-      <c r="D42" s="80"/>
+      <c r="D42" s="84"/>
       <c r="E42" s="40">
         <v>3</v>
       </c>
@@ -3720,11 +3727,11 @@
       <c r="B43" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C43" s="80">
+      <c r="C43" s="84">
         <f>C39*0.02</f>
         <v>10000</v>
       </c>
-      <c r="D43" s="80"/>
+      <c r="D43" s="84"/>
       <c r="E43" s="40">
         <v>2</v>
       </c>
@@ -3806,13 +3813,6 @@
     <row r="100" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C42:D42"/>
     <mergeCell ref="C43:D43"/>
     <mergeCell ref="A7:F7"/>
@@ -3821,6 +3821,13 @@
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="C41:D41"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
@@ -3831,4 +3838,1070 @@
     <brk id="28" max="10" man="1"/>
   </rowBreaks>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S99"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="33.77734375" customWidth="1"/>
+    <col min="3" max="3" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" customWidth="1"/>
+    <col min="6" max="6" width="8" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" customWidth="1"/>
+    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="81" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+    </row>
+    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="82" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="82"/>
+    </row>
+    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="70" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="70"/>
+    </row>
+    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="70" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="70"/>
+    </row>
+    <row r="5" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A5" s="83" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="83"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="83"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="74" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="74"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="74"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="74"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="80" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" s="80"/>
+      <c r="J6" s="80"/>
+      <c r="K6" s="80"/>
+      <c r="O6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="85" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="85"/>
+      <c r="C7" s="85"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="85"/>
+      <c r="F7" s="85"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="86" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" s="86"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="86"/>
+    </row>
+    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="N8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="124.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="64">
+        <v>1</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+      <c r="N9" t="s">
+        <v>48</v>
+      </c>
+      <c r="O9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="18"/>
+      <c r="B10" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="37">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="39">
+        <f>D29</f>
+        <v>12.3</v>
+      </c>
+      <c r="E10" s="39">
+        <f>(F29/2)-0.1009</f>
+        <v>1.6491</v>
+      </c>
+      <c r="F10" s="39">
+        <f>2</f>
+        <v>2</v>
+      </c>
+      <c r="G10" s="40">
+        <f>PRODUCT(C10:F10)</f>
+        <v>20.283930000000002</v>
+      </c>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="21"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="25"/>
+      <c r="S10" s="25"/>
+    </row>
+    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="18"/>
+      <c r="B11" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="19"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="23">
+        <f>SUM(G10:G10)</f>
+        <v>20.283930000000002</v>
+      </c>
+      <c r="H11" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" s="23">
+        <v>736.88</v>
+      </c>
+      <c r="J11" s="42">
+        <f>G11*I11</f>
+        <v>14946.822338400001</v>
+      </c>
+      <c r="K11" s="21"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="25"/>
+      <c r="S11" s="25"/>
+    </row>
+    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="18"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="21"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="25"/>
+      <c r="S12" s="25"/>
+    </row>
+    <row r="13" spans="1:19" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="18">
+        <v>2</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="19"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="42"/>
+      <c r="K13" s="21"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="25"/>
+      <c r="S13" s="25"/>
+    </row>
+    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="18"/>
+      <c r="B14" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="37">
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="39">
+        <f>D18</f>
+        <v>12.3</v>
+      </c>
+      <c r="E14" s="39">
+        <v>1</v>
+      </c>
+      <c r="F14" s="39">
+        <v>1.5</v>
+      </c>
+      <c r="G14" s="40">
+        <f>PRODUCT(C14:F14)</f>
+        <v>9.2250000000000014</v>
+      </c>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="21"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="25"/>
+      <c r="S14" s="25"/>
+    </row>
+    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="18"/>
+      <c r="B15" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="19"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="23">
+        <f>SUM(G14:G14)</f>
+        <v>9.2250000000000014</v>
+      </c>
+      <c r="H15" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="I15" s="23">
+        <v>404.28</v>
+      </c>
+      <c r="J15" s="42">
+        <f>G15*I15</f>
+        <v>3729.4830000000002</v>
+      </c>
+      <c r="K15" s="21"/>
+      <c r="M15" s="25"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="25"/>
+      <c r="S15" s="25"/>
+    </row>
+    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="18"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="21"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="25"/>
+      <c r="S16" s="25"/>
+    </row>
+    <row r="17" spans="1:19" ht="69" x14ac:dyDescent="0.3">
+      <c r="A17" s="18">
+        <v>3</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="19"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="42"/>
+      <c r="K17" s="21"/>
+      <c r="M17" s="25"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="25"/>
+      <c r="S17" s="25"/>
+    </row>
+    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="18"/>
+      <c r="B18" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="37">
+        <v>1</v>
+      </c>
+      <c r="D18" s="39">
+        <f>D23</f>
+        <v>12.3</v>
+      </c>
+      <c r="E18" s="39">
+        <f>E23</f>
+        <v>1.75</v>
+      </c>
+      <c r="F18" s="39">
+        <v>0.15</v>
+      </c>
+      <c r="G18" s="40">
+        <f>PRODUCT(C18:F18)</f>
+        <v>3.2287500000000002</v>
+      </c>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="21"/>
+      <c r="M18" s="25"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="25"/>
+      <c r="S18" s="25"/>
+    </row>
+    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="41"/>
+      <c r="B19" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="43"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="34">
+        <f>SUM(G18:G18)</f>
+        <v>3.2287500000000002</v>
+      </c>
+      <c r="H19" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="I19" s="34">
+        <v>4561.53</v>
+      </c>
+      <c r="J19" s="45">
+        <f>G19*I19</f>
+        <v>14728.0399875</v>
+      </c>
+      <c r="K19" s="37"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A20" s="41"/>
+      <c r="B20" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="43"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="46">
+        <f>0.13*G19*(15452.6/5)</f>
+        <v>1297.2071385000002</v>
+      </c>
+      <c r="K20" s="37"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A21" s="41"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="44"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="37"/>
+    </row>
+    <row r="22" spans="1:19" ht="69" x14ac:dyDescent="0.3">
+      <c r="A22" s="18">
+        <v>4</v>
+      </c>
+      <c r="B22" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="19"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="21"/>
+      <c r="M22" s="25"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="25"/>
+      <c r="S22" s="25"/>
+    </row>
+    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="18"/>
+      <c r="B23" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="37">
+        <v>1</v>
+      </c>
+      <c r="D23" s="39">
+        <f>D29</f>
+        <v>12.3</v>
+      </c>
+      <c r="E23" s="39">
+        <f>F29/2</f>
+        <v>1.75</v>
+      </c>
+      <c r="F23" s="39">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G23" s="40">
+        <f>PRODUCT(C23:F23)</f>
+        <v>1.6143750000000001</v>
+      </c>
+      <c r="H23" s="41"/>
+      <c r="I23" s="41"/>
+      <c r="J23" s="41"/>
+      <c r="K23" s="21"/>
+      <c r="M23" s="25"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="25"/>
+      <c r="S23" s="25"/>
+    </row>
+    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="18"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="37">
+        <v>1</v>
+      </c>
+      <c r="D24" s="39">
+        <f>D23</f>
+        <v>12.3</v>
+      </c>
+      <c r="E24" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="F24" s="39">
+        <v>0.05</v>
+      </c>
+      <c r="G24" s="40">
+        <f>PRODUCT(C24:F24)</f>
+        <v>0.30750000000000005</v>
+      </c>
+      <c r="H24" s="41"/>
+      <c r="I24" s="41"/>
+      <c r="J24" s="41"/>
+      <c r="K24" s="21"/>
+      <c r="M24" s="25"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="25"/>
+      <c r="S24" s="25"/>
+    </row>
+    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="41"/>
+      <c r="B25" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="43"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="34">
+        <f>SUM(G23:G24)</f>
+        <v>1.9218750000000002</v>
+      </c>
+      <c r="H25" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="I25" s="34">
+        <v>10634.5</v>
+      </c>
+      <c r="J25" s="45">
+        <f>G25*I25</f>
+        <v>20438.179687500004</v>
+      </c>
+      <c r="K25" s="37"/>
+    </row>
+    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="41"/>
+      <c r="B26" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="43"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="44"/>
+      <c r="I26" s="44"/>
+      <c r="J26" s="46">
+        <f>0.13*G25*((114907.3+6135.3)/15)</f>
+        <v>2016.1158062500003</v>
+      </c>
+      <c r="K26" s="37"/>
+    </row>
+    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="41"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="46"/>
+      <c r="K27" s="37"/>
+    </row>
+    <row r="28" spans="1:19" s="1" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="64">
+        <v>5</v>
+      </c>
+      <c r="B28" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="65"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="40"/>
+      <c r="H28" s="40"/>
+      <c r="I28" s="40"/>
+      <c r="J28" s="46"/>
+      <c r="K28" s="29"/>
+    </row>
+    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="18"/>
+      <c r="B29" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="37">
+        <v>1</v>
+      </c>
+      <c r="D29" s="39">
+        <v>12.3</v>
+      </c>
+      <c r="E29" s="39">
+        <f>((F29/2+0.5)/2)-0.00000488889</f>
+        <v>1.1249951111100001</v>
+      </c>
+      <c r="F29" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="G29" s="40">
+        <f>PRODUCT(C29:F29)</f>
+        <v>48.431039533285507</v>
+      </c>
+      <c r="H29" s="41"/>
+      <c r="I29" s="41"/>
+      <c r="J29" s="41"/>
+      <c r="K29" s="21"/>
+      <c r="M29" s="25"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="25"/>
+      <c r="S29" s="25"/>
+    </row>
+    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="41"/>
+      <c r="B30" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="43"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="34">
+        <f>SUM(G29:G29)</f>
+        <v>48.431039533285507</v>
+      </c>
+      <c r="H30" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="I30" s="34">
+        <v>9623.4699999999993</v>
+      </c>
+      <c r="J30" s="45">
+        <f>G30*I30</f>
+        <v>466074.65601738705</v>
+      </c>
+      <c r="K30" s="37"/>
+    </row>
+    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="41"/>
+      <c r="B31" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="43"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="44"/>
+      <c r="G31" s="44"/>
+      <c r="H31" s="44"/>
+      <c r="I31" s="44"/>
+      <c r="J31" s="46">
+        <f>0.13*G30*((59609.3+3478.36)/10)</f>
+        <v>39720.212421792174</v>
+      </c>
+      <c r="K31" s="37"/>
+    </row>
+    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="41"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="44"/>
+      <c r="G32" s="34"/>
+      <c r="H32" s="34"/>
+      <c r="I32" s="34"/>
+      <c r="J32" s="45"/>
+      <c r="K32" s="37"/>
+    </row>
+    <row r="33" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="18">
+        <v>6</v>
+      </c>
+      <c r="B33" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="19">
+        <v>1</v>
+      </c>
+      <c r="D33" s="20"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="35">
+        <f t="shared" ref="G33" si="0">PRODUCT(C33:F33)</f>
+        <v>1</v>
+      </c>
+      <c r="H33" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I33" s="23">
+        <v>500</v>
+      </c>
+      <c r="J33" s="35">
+        <f>G33*I33</f>
+        <v>500</v>
+      </c>
+      <c r="K33" s="21"/>
+      <c r="M33" s="25"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="25"/>
+      <c r="S33" s="25"/>
+    </row>
+    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="18"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="42"/>
+      <c r="K34" s="21"/>
+      <c r="M34" s="25"/>
+      <c r="N34" s="1">
+        <f>2.4*3.281</f>
+        <v>7.8743999999999996</v>
+      </c>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="25"/>
+      <c r="S34" s="25"/>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A35" s="41"/>
+      <c r="B35" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="48"/>
+      <c r="D35" s="39"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="42"/>
+      <c r="H35" s="42"/>
+      <c r="I35" s="42"/>
+      <c r="J35" s="42">
+        <f>SUM(J10:J33)</f>
+        <v>563450.71639732923</v>
+      </c>
+      <c r="K35" s="37"/>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A36" s="59"/>
+      <c r="B36" s="62"/>
+      <c r="C36" s="63"/>
+      <c r="D36" s="60"/>
+      <c r="E36" s="60"/>
+      <c r="F36" s="60"/>
+      <c r="G36" s="61"/>
+      <c r="H36" s="61"/>
+      <c r="I36" s="61"/>
+      <c r="J36" s="61"/>
+      <c r="K36" s="58"/>
+    </row>
+    <row r="37" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="51"/>
+      <c r="B37" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C37" s="84">
+        <f>J35</f>
+        <v>563450.71639732923</v>
+      </c>
+      <c r="D37" s="84"/>
+      <c r="E37" s="40">
+        <v>100</v>
+      </c>
+      <c r="F37" s="52"/>
+      <c r="G37" s="53"/>
+      <c r="H37" s="52"/>
+      <c r="I37" s="54"/>
+      <c r="J37" s="55"/>
+      <c r="K37" s="56"/>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A38" s="57"/>
+      <c r="B38" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" s="87">
+        <v>500000</v>
+      </c>
+      <c r="D38" s="87"/>
+      <c r="E38" s="40"/>
+      <c r="F38" s="50"/>
+      <c r="G38" s="49"/>
+      <c r="H38" s="49"/>
+      <c r="I38" s="49"/>
+      <c r="J38" s="49"/>
+      <c r="K38" s="50"/>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A39" s="57"/>
+      <c r="B39" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39" s="87">
+        <f>C38-C41-C42</f>
+        <v>475000</v>
+      </c>
+      <c r="D39" s="87"/>
+      <c r="E39" s="40">
+        <f>C39/C37*100</f>
+        <v>84.301960433580078</v>
+      </c>
+      <c r="F39" s="50"/>
+      <c r="G39" s="49"/>
+      <c r="H39" s="49"/>
+      <c r="I39" s="49"/>
+      <c r="J39" s="49"/>
+      <c r="K39" s="50"/>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A40" s="57"/>
+      <c r="B40" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C40" s="84">
+        <f>C37-C39</f>
+        <v>88450.716397329234</v>
+      </c>
+      <c r="D40" s="84"/>
+      <c r="E40" s="40">
+        <f>100-E39</f>
+        <v>15.698039566419922</v>
+      </c>
+      <c r="F40" s="50"/>
+      <c r="G40" s="49"/>
+      <c r="H40" s="49"/>
+      <c r="I40" s="49"/>
+      <c r="J40" s="49"/>
+      <c r="K40" s="50"/>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A41" s="57"/>
+      <c r="B41" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C41" s="84">
+        <f>C38*0.03</f>
+        <v>15000</v>
+      </c>
+      <c r="D41" s="84"/>
+      <c r="E41" s="40">
+        <v>3</v>
+      </c>
+      <c r="F41" s="50"/>
+      <c r="G41" s="49"/>
+      <c r="H41" s="49"/>
+      <c r="I41" s="49"/>
+      <c r="J41" s="49"/>
+      <c r="K41" s="50"/>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A42" s="57"/>
+      <c r="B42" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C42" s="84">
+        <f>C38*0.02</f>
+        <v>10000</v>
+      </c>
+      <c r="D42" s="84"/>
+      <c r="E42" s="40">
+        <v>2</v>
+      </c>
+      <c r="F42" s="50"/>
+      <c r="G42" s="49"/>
+      <c r="H42" s="49"/>
+      <c r="I42" s="49"/>
+      <c r="J42" s="49"/>
+      <c r="K42" s="50"/>
+    </row>
+    <row r="43" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="58"/>
+      <c r="B43" s="58"/>
+      <c r="C43" s="58"/>
+      <c r="D43" s="58"/>
+      <c r="E43" s="58"/>
+      <c r="F43" s="58"/>
+      <c r="G43" s="58"/>
+      <c r="H43" s="58"/>
+      <c r="I43" s="58"/>
+      <c r="J43" s="58"/>
+      <c r="K43" s="58"/>
+    </row>
+    <row r="44" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="49" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="50" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="51" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="52" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="53" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="54" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="55" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="56" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="57" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="58" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="59" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="60" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="61" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="62" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="63" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="64" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="65" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="66" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="67" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="68" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="69" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="70" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="71" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="72" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="73" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="74" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="75" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="76" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="77" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="78" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="79" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="80" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="81" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="82" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="83" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="84" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="85" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="86" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="87" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="88" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="89" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="90" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="91" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="92" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="93" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="94" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="95" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="96" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="97" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="98" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="99" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+  </mergeCells>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="70" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LPrepared By:&amp;CChecked By:&amp;RApproved By:</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>